<commit_message>
JL/DY - #14 - update excel template
</commit_message>
<xml_diff>
--- a/modules/export/src/main/resources/templates/template_Simam_import_Requi.xlsx
+++ b/modules/export/src/main/resources/templates/template_Simam_import_Requi.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>CLiente</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>${quantity_approved}</t>
+  </si>
+  <si>
+    <t>${inventory}</t>
   </si>
 </sst>
 </file>
@@ -617,7 +620,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -693,7 +696,7 @@
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
DY - #496 - SIMAM email excel enhancement
</commit_message>
<xml_diff>
--- a/modules/export/src/main/resources/templates/template_Simam_import_Requi.xlsx
+++ b/modules/export/src/main/resources/templates/template_Simam_import_Requi.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>CLiente</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>${inventory}</t>
+  </si>
+  <si>
+    <t>${emprest}</t>
+  </si>
+  <si>
+    <t>${quantity_requested}</t>
   </si>
 </sst>
 </file>
@@ -620,7 +626,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -689,11 +695,17 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
       <c r="H2" t="s">
         <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>

</xml_diff>